<commit_message>
Trying to do git
</commit_message>
<xml_diff>
--- a/Data/Migration Map Data.xlsx
+++ b/Data/Migration Map Data.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="18" documentId="8_{5FC1E408-A01A-4A36-A813-C07D40C6E3CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B7FB2E39-D782-4D5C-851D-E5519E77D953}"/>
   <bookViews>
-    <workbookView xWindow="24600" yWindow="13380" windowWidth="18975" windowHeight="13155" xr2:uid="{0989B1F8-E95E-479E-8A3C-F17C8275F488}"/>
+    <workbookView xWindow="18270" yWindow="9915" windowWidth="26625" windowHeight="13155" xr2:uid="{0989B1F8-E95E-479E-8A3C-F17C8275F488}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -655,7 +655,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DDECC5-6D04-4C9B-9DE0-A6112A9F947E}">
   <dimension ref="A1:AL14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Merged anmd Cleaned up Deck into new version
</commit_message>
<xml_diff>
--- a/Data/Migration Map Data.xlsx
+++ b/Data/Migration Map Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxwelloteng/Desktop/DataClass/project_2/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evidant-my.sharepoint.com/personal/sdleslie_evidant_com/Documents/Education/UCI Data Boot Camp/Git Master/project_2/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC86CE3D-AC2C-6645-8B27-229B8C2AC1B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="6_{48356985-E46C-48BA-8845-4BE50B7E834C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{64364AC0-F06F-46E3-8187-1388BE672F60}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="520" windowWidth="40520" windowHeight="16680" activeTab="7" xr2:uid="{0989B1F8-E95E-479E-8A3C-F17C8275F488}"/>
+    <workbookView xWindow="11130" yWindow="6195" windowWidth="27975" windowHeight="17280" xr2:uid="{0989B1F8-E95E-479E-8A3C-F17C8275F488}"/>
   </bookViews>
   <sheets>
     <sheet name="original data" sheetId="1" r:id="rId1"/>
@@ -24,54 +24,26 @@
     <sheet name="age-gender-pyramid-chart" sheetId="6" r:id="rId9"/>
     <sheet name="workforce" sheetId="10" r:id="rId10"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'median income'!$A$2:$A$14</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'median income'!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Education attainment'!$E$49</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Education attainment'!$E$50:$E$62</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'Education attainment'!$F$49</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'Education attainment'!$F$50:$F$62</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'Education attainment'!$G$49</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'Education attainment'!$G$50:$G$62</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'Education attainment'!$H$49</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'Education attainment'!$H$50:$H$62</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'Education attainment'!$I$49</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'Education attainment'!$I$50:$I$62</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'median income'!$B$2:$B$14</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'Education attainment'!$B$50:$B$62</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'Education attainment'!$C$49</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'Education attainment'!$C$50:$C$62</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'Education attainment'!$D$49</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'Education attainment'!$D$50:$D$62</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'Education attainment'!$E$49</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'Education attainment'!$E$50:$E$62</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'Education attainment'!$F$49</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'Education attainment'!$F$50:$F$62</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">'Education attainment'!$G$49</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'median income'!$C$1</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">'Education attainment'!$G$50:$G$62</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">'Education attainment'!$H$49</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">'Education attainment'!$H$50:$H$62</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">'Education attainment'!$I$49</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">'Education attainment'!$I$50:$I$62</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'median income'!$C$2:$C$14</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Education attainment'!$B$50:$B$62</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Education attainment'!$C$49</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Education attainment'!$C$50:$C$62</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Education attainment'!$D$49</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Education attainment'!$D$50:$D$62</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="133">
   <si>
     <t>Mexico</t>
   </si>
@@ -469,6 +441,12 @@
   <si>
     <t>USA</t>
   </si>
+  <si>
+    <t>Full Time</t>
+  </si>
+  <si>
+    <t>Part Time</t>
+  </si>
 </sst>
 </file>
 
@@ -481,7 +459,7 @@
     <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1026,7 +1004,19 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1037,18 +1027,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3987,14 +3965,16 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1600"/>
-              <a:t>Demographics:</a:t>
+              <a:rPr lang="en-US" sz="2000" baseline="0">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Median Income by Birth Country</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" baseline="0"/>
-              <a:t> Median Income by Region of Birth</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1600"/>
+            <a:endParaRPr lang="en-US" sz="2000">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4002,8 +3982,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.36673233994961535"/>
-          <c:y val="1.2903225806451613E-2"/>
+          <c:x val="0.39738063870420864"/>
+          <c:y val="2.5806451612903226E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4037,7 +4017,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.24579331429725129"/>
+          <c:y val="0.11096774193548387"/>
+          <c:w val="0.61103187393404623"/>
+          <c:h val="0.82916576073152148"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="stacked"/>
@@ -4051,7 +4041,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> Median_Income_FT </c:v>
+                  <c:v> Full Time </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4176,7 +4166,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> Median_Income_PT </c:v>
+                  <c:v> Part Time </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4334,16 +4324,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -4390,16 +4380,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -4423,10 +4413,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.85770828861600334"/>
-          <c:y val="0.2093994411988824"/>
-          <c:w val="0.13428668567379609"/>
-          <c:h val="8.6195891964264346E-2"/>
+          <c:x val="0.86900587975953558"/>
+          <c:y val="7.26252476504953E-2"/>
+          <c:w val="9.8917909986526414E-2"/>
+          <c:h val="0.10942179324358649"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4442,16 +4432,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -19063,16 +19053,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19666,49 +19656,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DDECC5-6D04-4C9B-9DE0-A6112A9F947E}">
   <dimension ref="A1:AL14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:AA10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="93" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="93" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="93" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="93" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="93" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="93" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="93" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="93" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="93" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="93" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" style="94" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" style="93" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" style="93" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" style="93" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="14.1640625" style="93" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" style="93" hidden="1" customWidth="1"/>
-    <col min="15" max="17" width="17.5" style="93" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="16.33203125" style="93" hidden="1" customWidth="1"/>
-    <col min="19" max="21" width="17.1640625" style="93" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="93" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="93" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="93" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="93" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="94" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="93" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" style="93" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" style="93" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" style="93" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" style="93" hidden="1" customWidth="1"/>
+    <col min="15" max="17" width="17.42578125" style="93" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="16.28515625" style="93" hidden="1" customWidth="1"/>
+    <col min="19" max="21" width="17.140625" style="93" customWidth="1"/>
     <col min="22" max="23" width="15" style="93" customWidth="1"/>
-    <col min="24" max="24" width="16.33203125" style="93" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.28515625" style="93" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="20" style="93" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.5" style="93" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.42578125" style="93" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" style="93" customWidth="1"/>
-    <col min="28" max="28" width="15.5" style="93" customWidth="1"/>
-    <col min="29" max="29" width="22.33203125" style="93" customWidth="1"/>
-    <col min="30" max="30" width="13.83203125" style="93" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5" style="93" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.83203125" style="93" customWidth="1"/>
-    <col min="33" max="33" width="16.5" style="93" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.33203125" style="93" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.42578125" style="93" customWidth="1"/>
+    <col min="29" max="29" width="22.28515625" style="93" customWidth="1"/>
+    <col min="30" max="30" width="13.85546875" style="93" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="93" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.85546875" style="93" customWidth="1"/>
+    <col min="33" max="33" width="16.42578125" style="93" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.28515625" style="93" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14" style="93" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.1640625" style="93" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.140625" style="93" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="9" style="93" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="13" style="93" customWidth="1"/>
-    <col min="39" max="16384" width="9.1640625" style="93"/>
+    <col min="39" max="16384" width="9.140625" style="93"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="90" customFormat="1" ht="18.75" customHeight="1">
+    <row r="1" spans="1:38" s="90" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
         <v>43</v>
       </c>
@@ -19824,7 +19814,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="101" t="s">
         <v>12</v>
       </c>
@@ -19930,7 +19920,7 @@
         <v>1317281</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="101" t="s">
         <v>0</v>
       </c>
@@ -20046,7 +20036,7 @@
         <v>68478</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="101" t="s">
         <v>1</v>
       </c>
@@ -20162,7 +20152,7 @@
         <v>39188</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="101" t="s">
         <v>2</v>
       </c>
@@ -20276,7 +20266,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="101" t="s">
         <v>3</v>
       </c>
@@ -20392,7 +20382,7 @@
         <v>24066</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="101" t="s">
         <v>4</v>
       </c>
@@ -20506,7 +20496,7 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="101" t="s">
         <v>5</v>
       </c>
@@ -20622,7 +20612,7 @@
         <v>15986</v>
       </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="101" t="s">
         <v>6</v>
       </c>
@@ -20738,7 +20728,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="101" t="s">
         <v>7</v>
       </c>
@@ -20854,7 +20844,7 @@
         <v>38632</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="101" t="s">
         <v>8</v>
       </c>
@@ -20968,7 +20958,7 @@
         <v>21807</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="101" t="s">
         <v>9</v>
       </c>
@@ -21084,7 +21074,7 @@
         <v>15344</v>
       </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="101" t="s">
         <v>10</v>
       </c>
@@ -21200,7 +21190,7 @@
         <v>14942</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="101" t="s">
         <v>11</v>
       </c>
@@ -21331,9 +21321,9 @@
       <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" ht="32">
+    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
@@ -21386,7 +21376,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -21439,7 +21429,7 @@
         <v>68478</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -21492,7 +21482,7 @@
         <v>39188</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -21545,7 +21535,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -21598,7 +21588,7 @@
         <v>24066</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -21651,7 +21641,7 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -21704,7 +21694,7 @@
         <v>15986</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -21757,7 +21747,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -21810,7 +21800,7 @@
         <v>38632</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -21863,7 +21853,7 @@
         <v>21807</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -21916,7 +21906,7 @@
         <v>15344</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
@@ -21969,7 +21959,7 @@
         <v>14942</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -22022,7 +22012,7 @@
         <v>16584</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -22041,7 +22031,7 @@
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
     </row>
-    <row r="15" spans="1:17" ht="32">
+    <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -22091,7 +22081,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>130</v>
       </c>
@@ -22158,9 +22148,9 @@
       <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
@@ -22180,7 +22170,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -22200,7 +22190,7 @@
         <v>361893</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -22220,7 +22210,7 @@
         <v>930333</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -22240,7 +22230,7 @@
         <v>10376</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -22260,7 +22250,7 @@
         <v>628139</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -22280,7 +22270,7 @@
         <v>28837</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -22300,7 +22290,7 @@
         <v>636009</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -22320,7 +22310,7 @@
         <v>135332</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -22340,7 +22330,7 @@
         <v>253729</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -22360,7 +22350,7 @@
         <v>142635</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -22380,7 +22370,7 @@
         <v>251520</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -22400,7 +22390,7 @@
         <v>194614</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -22420,7 +22410,7 @@
         <v>140541</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
@@ -22440,7 +22430,7 @@
         <v>20231215</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>43</v>
       </c>
@@ -22460,7 +22450,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>0</v>
       </c>
@@ -22483,7 +22473,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>1</v>
       </c>
@@ -22506,7 +22496,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>2</v>
       </c>
@@ -22529,7 +22519,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="9"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>3</v>
       </c>
@@ -22552,7 +22542,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="9"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>4</v>
       </c>
@@ -22575,7 +22565,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>5</v>
       </c>
@@ -22598,7 +22588,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="9"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
@@ -22621,7 +22611,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
@@ -22644,7 +22634,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>8</v>
       </c>
@@ -22667,7 +22657,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="9"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>9</v>
       </c>
@@ -22690,7 +22680,7 @@
       <c r="H31" s="4"/>
       <c r="I31" s="9"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>10</v>
       </c>
@@ -22713,7 +22703,7 @@
       <c r="H32" s="4"/>
       <c r="I32" s="9"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>11</v>
       </c>
@@ -22745,29 +22735,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC16B50-6887-2546-98B9-F580222B7FFA}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -22778,7 +22768,7 @@
         <v>-35000</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -22789,7 +22779,7 @@
         <v>-26000</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -22800,7 +22790,7 @@
         <v>-39000</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -22811,7 +22801,7 @@
         <v>-32000</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -22822,7 +22812,7 @@
         <v>-62000</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -22833,7 +22823,7 @@
         <v>-40000</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -22844,7 +22834,7 @@
         <v>-48600</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -22855,7 +22845,7 @@
         <v>-56000</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -22866,7 +22856,7 @@
         <v>-29400</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -22877,7 +22867,7 @@
         <v>-25200</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -22888,7 +22878,7 @@
         <v>-31200</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -22899,7 +22889,7 @@
         <v>-40000</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -22908,16 +22898,6 @@
       </c>
       <c r="C14" s="4">
         <v>-32000</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4">
-      <c r="D17">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4">
-      <c r="C18">
-        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -22935,9 +22915,9 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22" defaultRowHeight="17.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="22" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.25" customHeight="1">
+    <row r="1" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -22978,7 +22958,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17.25" customHeight="1">
+    <row r="2" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -23019,7 +22999,7 @@
         <v>141661</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17.25" customHeight="1">
+    <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -23060,7 +23040,7 @@
         <v>92680</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17.25" customHeight="1">
+    <row r="4" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -23101,7 +23081,7 @@
         <v>44282</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17.25" customHeight="1">
+    <row r="5" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -23142,7 +23122,7 @@
         <v>81342</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="17.25" customHeight="1">
+    <row r="6" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -23183,7 +23163,7 @@
         <v>335065</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17.25" customHeight="1">
+    <row r="7" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -23224,7 +23204,7 @@
         <v>66173</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="17.25" customHeight="1">
+    <row r="8" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
@@ -23265,7 +23245,7 @@
         <v>68446</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="17.25" customHeight="1">
+    <row r="9" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -23306,7 +23286,7 @@
         <v>77875</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="17.25" customHeight="1">
+    <row r="10" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -23347,7 +23327,7 @@
         <v>116271</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="17.25" customHeight="1">
+    <row r="11" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -23388,7 +23368,7 @@
         <v>121349</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="17.25" customHeight="1">
+    <row r="12" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -23429,7 +23409,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="17.25" customHeight="1">
+    <row r="13" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -23470,7 +23450,7 @@
         <v>22537</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="17.25" customHeight="1">
+    <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -23511,7 +23491,7 @@
         <v>107910</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="17.25" customHeight="1">
+    <row r="15" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -23552,7 +23532,7 @@
         <v>193221</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="17.25" customHeight="1">
+    <row r="16" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -23593,7 +23573,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="17.25" customHeight="1">
+    <row r="17" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>30</v>
       </c>
@@ -23634,7 +23614,7 @@
         <v>16584</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="17.25" customHeight="1">
+    <row r="19" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -23687,7 +23667,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="17.25" customHeight="1">
+    <row r="20" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6">
         <v>20010377</v>
       </c>
@@ -23737,7 +23717,7 @@
         <v>1317281</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="17.25" customHeight="1">
+    <row r="21" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -23790,7 +23770,7 @@
         <v>68478</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="17.25" customHeight="1">
+    <row r="22" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -23843,7 +23823,7 @@
         <v>39188</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="17.25" customHeight="1">
+    <row r="23" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -23896,7 +23876,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="17.25" customHeight="1">
+    <row r="24" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -23949,7 +23929,7 @@
         <v>24066</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="17.25" customHeight="1">
+    <row r="25" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -24002,7 +23982,7 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="17.25" customHeight="1">
+    <row r="26" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -24055,7 +24035,7 @@
         <v>15986</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="17.25" customHeight="1">
+    <row r="27" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -24108,7 +24088,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="17.25" customHeight="1">
+    <row r="28" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -24161,7 +24141,7 @@
         <v>38632</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="17.25" customHeight="1">
+    <row r="29" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -24214,7 +24194,7 @@
         <v>21807</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="17.25" customHeight="1">
+    <row r="30" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -24267,7 +24247,7 @@
         <v>15344</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="17.25" customHeight="1">
+    <row r="31" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -24320,7 +24300,7 @@
         <v>14942</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="17.25" customHeight="1">
+    <row r="32" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -24373,82 +24353,82 @@
         <v>16584</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="17.25" customHeight="1">
+    <row r="35" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>20010377</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="17.25" customHeight="1">
+    <row r="36" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>8318530</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="17.25" customHeight="1">
+    <row r="37" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>4578675</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="17.25" customHeight="1">
+    <row r="38" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>13573179</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="17.25" customHeight="1">
+    <row r="39" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>13995427</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="17.25" customHeight="1">
+    <row r="40" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>9570999</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="17.25" customHeight="1">
+    <row r="41" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>4183259</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="17.25" customHeight="1">
+    <row r="42" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>8377235</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="17.25" customHeight="1">
+    <row r="43" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>17391363</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="17.25" customHeight="1">
+    <row r="44" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>19613568</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="17.25" customHeight="1">
+    <row r="45" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>916886</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="17.25" customHeight="1">
+    <row r="46" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>7269547</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="17.25" customHeight="1">
+    <row r="47" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>11784060</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="17.25" customHeight="1">
+    <row r="48" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>12504870</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="17.25" customHeight="1">
+    <row r="49" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>556905</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="17.25" customHeight="1">
+    <row r="50" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>1317281</v>
       </c>
@@ -24467,9 +24447,9 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
@@ -24489,7 +24469,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -24509,7 +24489,7 @@
         <v>5753368</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -24529,7 +24509,7 @@
         <v>4334258</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -24549,7 +24529,7 @@
         <v>34239</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -24569,7 +24549,7 @@
         <v>1013222</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -24589,7 +24569,7 @@
         <v>89888</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -24609,7 +24589,7 @@
         <v>2783356</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -24629,7 +24609,7 @@
         <v>457984</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -24649,7 +24629,7 @@
         <v>2169302</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -24669,7 +24649,7 @@
         <v>1469200</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -24689,7 +24669,7 @@
         <v>1311556</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
@@ -24709,7 +24689,7 @@
         <v>686733</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -24743,13 +24723,13 @@
       <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>43</v>
       </c>
@@ -24781,7 +24761,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="2:12">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
@@ -24817,7 +24797,7 @@
         <v>203441977</v>
       </c>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -24853,7 +24833,7 @@
         <v>10462474</v>
       </c>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -24889,7 +24869,7 @@
         <v>8435502</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -24923,7 +24903,7 @@
         <v>114452</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
@@ -24959,7 +24939,7 @@
         <v>3474289</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
@@ -24993,7 +24973,7 @@
         <v>227430</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
@@ -25029,7 +25009,7 @@
         <v>4684644</v>
       </c>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
@@ -25065,7 +25045,7 @@
         <v>800212</v>
       </c>
     </row>
-    <row r="10" spans="2:12">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
@@ -25101,7 +25081,7 @@
         <v>4216030</v>
       </c>
     </row>
-    <row r="11" spans="2:12">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
@@ -25135,7 +25115,7 @@
         <v>3116026</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
@@ -25171,7 +25151,7 @@
         <v>3161060</v>
       </c>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
@@ -25207,7 +25187,7 @@
         <v>1720770</v>
       </c>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
@@ -25243,7 +25223,7 @@
         <v>1925582</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>43</v>
       </c>
@@ -25275,7 +25255,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="2:12">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>12</v>
       </c>
@@ -25311,7 +25291,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>0</v>
       </c>
@@ -25347,7 +25327,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>1</v>
       </c>
@@ -25383,7 +25363,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:12">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>2</v>
       </c>
@@ -25419,7 +25399,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="2:12">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>3</v>
       </c>
@@ -25455,7 +25435,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="2:12">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>4</v>
       </c>
@@ -25491,7 +25471,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="2:12">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>5</v>
       </c>
@@ -25527,7 +25507,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="2:12">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>6</v>
       </c>
@@ -25563,7 +25543,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="2:12">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>7</v>
       </c>
@@ -25599,7 +25579,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="2:12">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>8</v>
       </c>
@@ -25635,7 +25615,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="2:12">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>9</v>
       </c>
@@ -25671,7 +25651,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="2:12">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>10</v>
       </c>
@@ -25707,7 +25687,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="2:12">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>11</v>
       </c>
@@ -25743,7 +25723,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="2:10">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>43</v>
       </c>
@@ -25772,7 +25752,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="2:10">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>12</v>
       </c>
@@ -25801,7 +25781,7 @@
         <v>184555298</v>
       </c>
     </row>
-    <row r="36" spans="2:10">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>0</v>
       </c>
@@ -25830,7 +25810,7 @@
         <v>10069030</v>
       </c>
     </row>
-    <row r="37" spans="2:10">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>1</v>
       </c>
@@ -25859,7 +25839,7 @@
         <v>7618548</v>
       </c>
     </row>
-    <row r="38" spans="2:10">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
         <v>2</v>
       </c>
@@ -25886,7 +25866,7 @@
         <v>101852</v>
       </c>
     </row>
-    <row r="39" spans="2:10">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>3</v>
       </c>
@@ -25915,7 +25895,7 @@
         <v>3168503</v>
       </c>
     </row>
-    <row r="40" spans="2:10">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
         <v>4</v>
       </c>
@@ -25942,7 +25922,7 @@
         <v>209306</v>
       </c>
     </row>
-    <row r="41" spans="2:10">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
         <v>5</v>
       </c>
@@ -25971,7 +25951,7 @@
         <v>4413581</v>
       </c>
     </row>
-    <row r="42" spans="2:10">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
         <v>6</v>
       </c>
@@ -26000,7 +25980,7 @@
         <v>745687</v>
       </c>
     </row>
-    <row r="43" spans="2:10">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
         <v>7</v>
       </c>
@@ -26029,7 +26009,7 @@
         <v>3927095</v>
       </c>
     </row>
-    <row r="44" spans="2:10">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
         <v>8</v>
       </c>
@@ -26058,7 +26038,7 @@
         <v>3031989</v>
       </c>
     </row>
-    <row r="45" spans="2:10">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>9</v>
       </c>
@@ -26087,7 +26067,7 @@
         <v>2897536</v>
       </c>
     </row>
-    <row r="46" spans="2:10">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
         <v>10</v>
       </c>
@@ -26116,7 +26096,7 @@
         <v>1523236</v>
       </c>
     </row>
-    <row r="47" spans="2:10">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
         <v>11</v>
       </c>
@@ -26145,7 +26125,7 @@
         <v>1617749</v>
       </c>
     </row>
-    <row r="49" spans="2:10">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>43</v>
       </c>
@@ -26174,7 +26154,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="2:10">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
         <v>12</v>
       </c>
@@ -26203,7 +26183,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:10">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>0</v>
       </c>
@@ -26232,7 +26212,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="2:10">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>1</v>
       </c>
@@ -26261,7 +26241,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="2:10">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>2</v>
       </c>
@@ -26290,7 +26270,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="2:10">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>3</v>
       </c>
@@ -26319,7 +26299,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="2:10">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
         <v>4</v>
       </c>
@@ -26348,7 +26328,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="2:10">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
         <v>5</v>
       </c>
@@ -26377,7 +26357,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="2:10">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
         <v>6</v>
       </c>
@@ -26406,7 +26386,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="2:10">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
         <v>7</v>
       </c>
@@ -26435,7 +26415,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="2:10">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="s">
         <v>8</v>
       </c>
@@ -26464,7 +26444,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="2:10">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B60" s="4" t="s">
         <v>9</v>
       </c>
@@ -26493,7 +26473,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="2:10">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
         <v>10</v>
       </c>
@@ -26522,7 +26502,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="2:10">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
         <v>11</v>
       </c>
@@ -26566,54 +26546,54 @@
       <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16">
-      <c r="A1" s="108" t="s">
+    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="104" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="108"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
       <c r="M1" s="24"/>
       <c r="N1" s="24"/>
     </row>
-    <row r="2" spans="1:14" ht="16">
-      <c r="A2" s="109" t="s">
+    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="105" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="109"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
       <c r="M2" s="24"/>
       <c r="N2" s="24"/>
     </row>
-    <row r="3" spans="1:14" ht="17">
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="60"/>
       <c r="B3" s="61" t="s">
         <v>112</v>
@@ -26630,18 +26610,18 @@
       <c r="H3" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="I3" s="103" t="s">
+      <c r="I3" s="106" t="s">
         <v>116</v>
       </c>
-      <c r="J3" s="103"/>
-      <c r="K3" s="103" t="s">
+      <c r="J3" s="106"/>
+      <c r="K3" s="106" t="s">
         <v>117</v>
       </c>
-      <c r="L3" s="103"/>
+      <c r="L3" s="106"/>
       <c r="M3" s="62"/>
       <c r="N3" s="24"/>
     </row>
-    <row r="4" spans="1:14" ht="51">
+    <row r="4" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
       <c r="B4" s="61" t="s">
         <v>118</v>
@@ -26658,20 +26638,20 @@
       <c r="H4" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="I4" s="103" t="s">
+      <c r="I4" s="106" t="s">
         <v>122</v>
       </c>
-      <c r="J4" s="103"/>
-      <c r="K4" s="110" t="s">
+      <c r="J4" s="106"/>
+      <c r="K4" s="107" t="s">
         <v>123</v>
       </c>
-      <c r="L4" s="110"/>
-      <c r="M4" s="103" t="s">
+      <c r="L4" s="107"/>
+      <c r="M4" s="106" t="s">
         <v>105</v>
       </c>
-      <c r="N4" s="103"/>
-    </row>
-    <row r="5" spans="1:14" ht="17">
+      <c r="N4" s="106"/>
+    </row>
+    <row r="5" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>124</v>
       </c>
@@ -26703,7 +26683,7 @@
         <v>282406817</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="34">
+    <row r="6" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>125</v>
       </c>
@@ -26735,7 +26715,7 @@
         <v>44760622</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17">
+    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="67" t="s">
         <v>0</v>
       </c>
@@ -26767,7 +26747,7 @@
         <v>11182111</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="51">
+    <row r="8" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="67" t="s">
         <v>1</v>
       </c>
@@ -26799,7 +26779,7 @@
         <v>8648528</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="34">
+    <row r="9" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="67" t="s">
         <v>2</v>
       </c>
@@ -26831,7 +26811,7 @@
         <v>131854</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17">
+    <row r="10" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="67" t="s">
         <v>3</v>
       </c>
@@ -26863,7 +26843,7 @@
         <v>3668982</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="17">
+    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="67" t="s">
         <v>4</v>
       </c>
@@ -26895,7 +26875,7 @@
         <v>246371</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17">
+    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="67" t="s">
         <v>5</v>
       </c>
@@ -26927,7 +26907,7 @@
         <v>4848270</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="68">
+    <row r="13" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A13" s="67" t="s">
         <v>6</v>
       </c>
@@ -26959,7 +26939,7 @@
         <v>827093</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17">
+    <row r="14" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="67" t="s">
         <v>7</v>
       </c>
@@ -26991,7 +26971,7 @@
         <v>4463891</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="34">
+    <row r="15" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="67" t="s">
         <v>8</v>
       </c>
@@ -27023,7 +27003,7 @@
         <v>3590330</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="34">
+    <row r="16" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="67" t="s">
         <v>9</v>
       </c>
@@ -27055,7 +27035,7 @@
         <v>3304380</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="51">
+    <row r="17" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="67" t="s">
         <v>10</v>
       </c>
@@ -27087,7 +27067,7 @@
         <v>1784898</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="51">
+    <row r="18" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
         <v>11</v>
       </c>
@@ -27119,7 +27099,7 @@
         <v>2032470</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16">
+    <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="70" t="s">
         <v>105</v>
       </c>
@@ -27146,12 +27126,12 @@
       <c r="L19" s="72">
         <v>253894500</v>
       </c>
-      <c r="M19" s="104">
+      <c r="M19" s="108">
         <v>327167439</v>
       </c>
-      <c r="N19" s="104"/>
-    </row>
-    <row r="20" spans="1:14" ht="16">
+      <c r="N19" s="108"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="73"/>
       <c r="B20" s="74"/>
       <c r="C20" s="74"/>
@@ -27167,25 +27147,25 @@
       <c r="M20" s="24"/>
       <c r="N20" s="24"/>
     </row>
-    <row r="21" spans="1:14" ht="16">
-      <c r="A21" s="105" t="s">
+    <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="109" t="s">
         <v>126</v>
       </c>
-      <c r="B21" s="105"/>
-      <c r="C21" s="105"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="105"/>
-      <c r="F21" s="105"/>
-      <c r="G21" s="105"/>
-      <c r="H21" s="105"/>
-      <c r="I21" s="105"/>
-      <c r="J21" s="105"/>
-      <c r="K21" s="105"/>
-      <c r="L21" s="105"/>
+      <c r="B21" s="109"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="109"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="109"/>
+      <c r="J21" s="109"/>
+      <c r="K21" s="109"/>
+      <c r="L21" s="109"/>
       <c r="M21" s="24"/>
       <c r="N21" s="24"/>
     </row>
-    <row r="22" spans="1:14" ht="17">
+    <row r="22" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
         <v>124</v>
       </c>
@@ -27236,7 +27216,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="34">
+    <row r="23" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
         <v>125</v>
       </c>
@@ -27275,7 +27255,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="17">
+    <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="67" t="s">
         <v>0</v>
       </c>
@@ -27314,7 +27294,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="51">
+    <row r="25" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A25" s="67" t="s">
         <v>1</v>
       </c>
@@ -27353,7 +27333,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="34">
+    <row r="26" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="67" t="s">
         <v>2</v>
       </c>
@@ -27392,7 +27372,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="17">
+    <row r="27" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="67" t="s">
         <v>3</v>
       </c>
@@ -27431,7 +27411,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="17">
+    <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="67" t="s">
         <v>4</v>
       </c>
@@ -27470,7 +27450,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="17">
+    <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="67" t="s">
         <v>5</v>
       </c>
@@ -27509,7 +27489,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="68">
+    <row r="30" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A30" s="67" t="s">
         <v>6</v>
       </c>
@@ -27548,7 +27528,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="17">
+    <row r="31" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="67" t="s">
         <v>7</v>
       </c>
@@ -27587,7 +27567,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="34">
+    <row r="32" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="67" t="s">
         <v>8</v>
       </c>
@@ -27626,7 +27606,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="34">
+    <row r="33" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="67" t="s">
         <v>9</v>
       </c>
@@ -27665,7 +27645,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="51">
+    <row r="34" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A34" s="67" t="s">
         <v>10</v>
       </c>
@@ -27704,7 +27684,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="51">
+    <row r="35" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A35" s="80" t="s">
         <v>11</v>
       </c>
@@ -27743,7 +27723,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="17">
+    <row r="36" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="82" t="s">
         <v>127</v>
       </c>
@@ -27794,7 +27774,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16">
+    <row r="37" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="82"/>
       <c r="B37" s="83"/>
       <c r="C37" s="83"/>
@@ -27810,61 +27790,61 @@
       <c r="M37" s="57"/>
       <c r="N37" s="24"/>
     </row>
-    <row r="38" spans="1:14" ht="16">
-      <c r="A38" s="106" t="s">
+    <row r="38" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="106"/>
-      <c r="C38" s="106"/>
-      <c r="D38" s="106"/>
-      <c r="E38" s="106"/>
-      <c r="F38" s="106"/>
-      <c r="G38" s="106"/>
-      <c r="H38" s="106"/>
-      <c r="I38" s="106"/>
-      <c r="J38" s="106"/>
-      <c r="K38" s="106"/>
-      <c r="L38" s="106"/>
-      <c r="M38" s="106"/>
-      <c r="N38" s="106"/>
-    </row>
-    <row r="39" spans="1:14" ht="16">
-      <c r="A39" s="107" t="s">
+      <c r="B38" s="110"/>
+      <c r="C38" s="110"/>
+      <c r="D38" s="110"/>
+      <c r="E38" s="110"/>
+      <c r="F38" s="110"/>
+      <c r="G38" s="110"/>
+      <c r="H38" s="110"/>
+      <c r="I38" s="110"/>
+      <c r="J38" s="110"/>
+      <c r="K38" s="110"/>
+      <c r="L38" s="110"/>
+      <c r="M38" s="110"/>
+      <c r="N38" s="110"/>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="103" t="s">
         <v>106</v>
       </c>
-      <c r="B39" s="107"/>
-      <c r="C39" s="107"/>
-      <c r="D39" s="107"/>
-      <c r="E39" s="107"/>
-      <c r="F39" s="107"/>
-      <c r="G39" s="107"/>
-      <c r="H39" s="107"/>
-      <c r="I39" s="107"/>
-      <c r="J39" s="107"/>
-      <c r="K39" s="107"/>
-      <c r="L39" s="107"/>
+      <c r="B39" s="103"/>
+      <c r="C39" s="103"/>
+      <c r="D39" s="103"/>
+      <c r="E39" s="103"/>
+      <c r="F39" s="103"/>
+      <c r="G39" s="103"/>
+      <c r="H39" s="103"/>
+      <c r="I39" s="103"/>
+      <c r="J39" s="103"/>
+      <c r="K39" s="103"/>
+      <c r="L39" s="103"/>
       <c r="M39" s="24"/>
       <c r="N39" s="24"/>
     </row>
-    <row r="40" spans="1:14" ht="16">
-      <c r="A40" s="107" t="s">
+    <row r="40" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="103" t="s">
         <v>107</v>
       </c>
-      <c r="B40" s="107"/>
-      <c r="C40" s="107"/>
-      <c r="D40" s="107"/>
-      <c r="E40" s="107"/>
-      <c r="F40" s="107"/>
-      <c r="G40" s="107"/>
-      <c r="H40" s="107"/>
-      <c r="I40" s="107"/>
-      <c r="J40" s="107"/>
-      <c r="K40" s="107"/>
-      <c r="L40" s="107"/>
+      <c r="B40" s="103"/>
+      <c r="C40" s="103"/>
+      <c r="D40" s="103"/>
+      <c r="E40" s="103"/>
+      <c r="F40" s="103"/>
+      <c r="G40" s="103"/>
+      <c r="H40" s="103"/>
+      <c r="I40" s="103"/>
+      <c r="J40" s="103"/>
+      <c r="K40" s="103"/>
+      <c r="L40" s="103"/>
       <c r="M40" s="84"/>
       <c r="N40" s="24"/>
     </row>
-    <row r="41" spans="1:14" ht="51">
+    <row r="41" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A41" s="85" t="s">
         <v>108</v>
       </c>
@@ -27884,6 +27864,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A38:N38"/>
+    <mergeCell ref="A39:L39"/>
     <mergeCell ref="A40:L40"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
@@ -27891,11 +27876,6 @@
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A38:N38"/>
-    <mergeCell ref="A39:L39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -27906,39 +27886,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DCC33E2-2539-CD43-AC4A-8F37F5D6240C}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65:E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16">
-      <c r="A1" s="108" t="s">
+    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="104" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
       <c r="N1" s="24"/>
     </row>
-    <row r="2" spans="1:14" ht="16">
+    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="113" t="s">
         <v>75</v>
       </c>
@@ -27956,7 +27936,7 @@
       <c r="M2" s="113"/>
       <c r="N2" s="24"/>
     </row>
-    <row r="3" spans="1:14" ht="16">
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
       <c r="B3" s="114" t="s">
         <v>76</v>
@@ -27976,7 +27956,7 @@
       <c r="M3" s="115"/>
       <c r="N3" s="115"/>
     </row>
-    <row r="4" spans="1:14" ht="17">
+    <row r="4" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>78</v>
       </c>
@@ -28010,7 +27990,7 @@
       </c>
       <c r="N4" s="117"/>
     </row>
-    <row r="5" spans="1:14" ht="34">
+    <row r="5" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>83</v>
       </c>
@@ -28052,7 +28032,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17">
+    <row r="6" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>85</v>
       </c>
@@ -28086,7 +28066,7 @@
       </c>
       <c r="N6" s="37"/>
     </row>
-    <row r="7" spans="1:14" ht="34">
+    <row r="7" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>86</v>
       </c>
@@ -28124,7 +28104,7 @@
       </c>
       <c r="N7" s="44"/>
     </row>
-    <row r="8" spans="1:14" ht="17">
+    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>87</v>
       </c>
@@ -28162,7 +28142,7 @@
       </c>
       <c r="N8" s="44"/>
     </row>
-    <row r="9" spans="1:14" ht="17">
+    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>88</v>
       </c>
@@ -28200,7 +28180,7 @@
       </c>
       <c r="N9" s="44"/>
     </row>
-    <row r="10" spans="1:14" ht="17">
+    <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>89</v>
       </c>
@@ -28238,7 +28218,7 @@
       </c>
       <c r="N10" s="44"/>
     </row>
-    <row r="11" spans="1:14" ht="17">
+    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
         <v>90</v>
       </c>
@@ -28276,7 +28256,7 @@
       </c>
       <c r="N11" s="44"/>
     </row>
-    <row r="12" spans="1:14" ht="17">
+    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
         <v>91</v>
       </c>
@@ -28314,7 +28294,7 @@
       </c>
       <c r="N12" s="44"/>
     </row>
-    <row r="13" spans="1:14" ht="17">
+    <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
         <v>92</v>
       </c>
@@ -28352,7 +28332,7 @@
       </c>
       <c r="N13" s="44"/>
     </row>
-    <row r="14" spans="1:14" ht="17">
+    <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
         <v>93</v>
       </c>
@@ -28390,7 +28370,7 @@
       </c>
       <c r="N14" s="44"/>
     </row>
-    <row r="15" spans="1:14" ht="17">
+    <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
         <v>94</v>
       </c>
@@ -28428,7 +28408,7 @@
       </c>
       <c r="N15" s="44"/>
     </row>
-    <row r="16" spans="1:14" ht="17">
+    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
         <v>95</v>
       </c>
@@ -28466,7 +28446,7 @@
       </c>
       <c r="N16" s="44"/>
     </row>
-    <row r="17" spans="1:14" ht="17">
+    <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
         <v>96</v>
       </c>
@@ -28504,7 +28484,7 @@
       </c>
       <c r="N17" s="44"/>
     </row>
-    <row r="18" spans="1:14" ht="17">
+    <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>97</v>
       </c>
@@ -28542,7 +28522,7 @@
       </c>
       <c r="N18" s="44"/>
     </row>
-    <row r="19" spans="1:14" ht="17">
+    <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
         <v>98</v>
       </c>
@@ -28580,7 +28560,7 @@
       </c>
       <c r="N19" s="44"/>
     </row>
-    <row r="20" spans="1:14" ht="17">
+    <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
         <v>99</v>
       </c>
@@ -28618,7 +28598,7 @@
       </c>
       <c r="N20" s="44"/>
     </row>
-    <row r="21" spans="1:14" ht="17">
+    <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
         <v>100</v>
       </c>
@@ -28656,7 +28636,7 @@
       </c>
       <c r="N21" s="44"/>
     </row>
-    <row r="22" spans="1:14" ht="17">
+    <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
         <v>101</v>
       </c>
@@ -28694,7 +28674,7 @@
       </c>
       <c r="N22" s="44"/>
     </row>
-    <row r="23" spans="1:14" ht="17">
+    <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
         <v>102</v>
       </c>
@@ -28732,7 +28712,7 @@
       </c>
       <c r="N23" s="44"/>
     </row>
-    <row r="24" spans="1:14" ht="17">
+    <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="38" t="s">
         <v>103</v>
       </c>
@@ -28770,7 +28750,7 @@
       </c>
       <c r="N24" s="44"/>
     </row>
-    <row r="25" spans="1:14" ht="17">
+    <row r="25" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="46" t="s">
         <v>104</v>
       </c>
@@ -28808,7 +28788,7 @@
       </c>
       <c r="N25" s="53"/>
     </row>
-    <row r="26" spans="1:14" ht="17">
+    <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="54" t="s">
         <v>105</v>
       </c>
@@ -28854,7 +28834,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="13"/>
       <c r="C27" s="14"/>
@@ -28870,7 +28850,7 @@
       <c r="M27" s="14"/>
       <c r="N27" s="16"/>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="111" t="s">
         <v>106</v>
       </c>
@@ -28888,7 +28868,7 @@
       <c r="M28" s="111"/>
       <c r="N28" s="17"/>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="111" t="s">
         <v>107</v>
       </c>
@@ -28906,7 +28886,7 @@
       <c r="M29" s="111"/>
       <c r="N29" s="111"/>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="112" t="s">
         <v>108</v>
       </c>
@@ -28952,9 +28932,9 @@
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="16">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -28966,7 +28946,7 @@
       </c>
       <c r="H1" s="18"/>
     </row>
-    <row r="2" spans="1:8" ht="16">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -28976,7 +28956,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:8" ht="16">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>129</v>
       </c>
@@ -28996,7 +28976,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>86</v>
       </c>
@@ -29019,7 +28999,7 @@
         <v>3.4878074490673505</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>87</v>
       </c>
@@ -29042,7 +29022,7 @@
         <v>3.4610704882524135</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>88</v>
       </c>
@@ -29065,7 +29045,7 @@
         <v>3.7490674313290389</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>89</v>
       </c>
@@ -29088,7 +29068,7 @@
         <v>3.6062638672068594</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>90</v>
       </c>
@@ -29111,7 +29091,7 @@
         <v>3.5464614864449255</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16">
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>91</v>
       </c>
@@ -29134,7 +29114,7 @@
         <v>3.6178737144294928</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>92</v>
       </c>
@@ -29157,7 +29137,7 @@
         <v>3.1789615050262761</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16">
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>93</v>
       </c>
@@ -29180,7 +29160,7 @@
         <v>3.019607703025101</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16">
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>94</v>
       </c>
@@ -29203,7 +29183,7 @@
         <v>2.7043766439958139</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16">
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>95</v>
       </c>
@@ -29226,7 +29206,7 @@
         <v>2.8357477645449332</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="16">
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>96</v>
       </c>
@@ -29249,7 +29229,7 @@
         <v>2.9208416735917533</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16">
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>97</v>
       </c>
@@ -29272,7 +29252,7 @@
         <v>3.104774910585816</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="16">
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>98</v>
       </c>
@@ -29295,7 +29275,7 @@
         <v>3.0016598359946816</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="16">
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>99</v>
       </c>
@@ -29318,7 +29298,7 @@
         <v>2.4681932518647383</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="16">
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>100</v>
       </c>
@@ -29341,7 +29321,7 @@
         <v>1.9200988338748213</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="16">
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>101</v>
       </c>
@@ -29364,7 +29344,7 @@
         <v>1.2928126306526093</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="16">
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>102</v>
       </c>
@@ -29387,7 +29367,7 @@
         <v>0.78717150797390278</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="16">
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>103</v>
       </c>
@@ -29410,7 +29390,7 @@
         <v>0.45186869550673769</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="16">
+    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>104</v>
       </c>
@@ -29433,7 +29413,7 @@
         <v>0.23670675060227034</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="16">
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F25" s="18" t="s">
         <v>129</v>
       </c>
@@ -29444,7 +29424,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="16">
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F26" s="20" t="s">
         <v>86</v>
       </c>
@@ -29455,7 +29435,7 @@
         <v>0.32693915647552885</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="16">
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F27" s="20" t="s">
         <v>87</v>
       </c>
@@ -29466,7 +29446,7 @@
         <v>0.74659373589580591</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="16">
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F28" s="20" t="s">
         <v>88</v>
       </c>
@@ -29477,7 +29457,7 @@
         <v>0.98443001976156641</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="16">
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F29" s="20" t="s">
         <v>89</v>
       </c>
@@ -29488,7 +29468,7 @@
         <v>1.6485963934996257</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="16">
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F30" s="20" t="s">
         <v>90</v>
       </c>
@@ -29499,7 +29479,7 @@
         <v>2.5433382047282542</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="16">
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F31" s="20" t="s">
         <v>91</v>
       </c>
@@ -29510,7 +29490,7 @@
         <v>3.60095532184517</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="16">
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F32" s="20" t="s">
         <v>92</v>
       </c>
@@ -29521,7 +29501,7 @@
         <v>4.7716517433560233</v>
       </c>
     </row>
-    <row r="33" spans="6:8" ht="16">
+    <row r="33" spans="6:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F33" s="20" t="s">
         <v>93</v>
       </c>
@@ -29532,7 +29512,7 @@
         <v>5.1106751823064478</v>
       </c>
     </row>
-    <row r="34" spans="6:8" ht="16">
+    <row r="34" spans="6:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F34" s="20" t="s">
         <v>94</v>
       </c>
@@ -29543,7 +29523,7 @@
         <v>5.178346270523229</v>
       </c>
     </row>
-    <row r="35" spans="6:8" ht="16">
+    <row r="35" spans="6:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F35" s="20" t="s">
         <v>95</v>
       </c>
@@ -29554,7 +29534,7 @@
         <v>4.9843141143123528</v>
       </c>
     </row>
-    <row r="36" spans="6:8" ht="16">
+    <row r="36" spans="6:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F36" s="20" t="s">
         <v>96</v>
       </c>
@@ -29565,7 +29545,7 @@
         <v>4.4710035530784173</v>
       </c>
     </row>
-    <row r="37" spans="6:8" ht="16">
+    <row r="37" spans="6:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F37" s="20" t="s">
         <v>97</v>
       </c>
@@ -29576,7 +29556,7 @@
         <v>3.8129362902955188</v>
       </c>
     </row>
-    <row r="38" spans="6:8" ht="16">
+    <row r="38" spans="6:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F38" s="20" t="s">
         <v>98</v>
       </c>
@@ -29587,7 +29567,7 @@
         <v>3.2087579122560004</v>
       </c>
     </row>
-    <row r="39" spans="6:8" ht="16">
+    <row r="39" spans="6:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F39" s="20" t="s">
         <v>99</v>
       </c>
@@ -29598,7 +29578,7 @@
         <v>2.4340970954335712</v>
       </c>
     </row>
-    <row r="40" spans="6:8" ht="16">
+    <row r="40" spans="6:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F40" s="20" t="s">
         <v>100</v>
       </c>
@@ -29609,7 +29589,7 @@
         <v>1.7795396140831108</v>
       </c>
     </row>
-    <row r="41" spans="6:8" ht="16">
+    <row r="41" spans="6:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F41" s="20" t="s">
         <v>101</v>
       </c>
@@ -29620,7 +29600,7 @@
         <v>1.1943332690953223</v>
       </c>
     </row>
-    <row r="42" spans="6:8" ht="16">
+    <row r="42" spans="6:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F42" s="20" t="s">
         <v>102</v>
       </c>
@@ -29631,7 +29611,7 @@
         <v>0.79006498167071937</v>
       </c>
     </row>
-    <row r="43" spans="6:8" ht="16">
+    <row r="43" spans="6:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F43" s="20" t="s">
         <v>103</v>
       </c>
@@ -29642,7 +29622,7 @@
         <v>0.41348397705465306</v>
       </c>
     </row>
-    <row r="44" spans="6:8" ht="16">
+    <row r="44" spans="6:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F44" s="20" t="s">
         <v>104</v>
       </c>

</xml_diff>